<commit_message>
Finalised game builds, added and removed bibliography about engagement, prepared obsidian for annotations
</commit_message>
<xml_diff>
--- a/questionnaire.xlsx
+++ b/questionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\uczelnia\magister\PRACA DYPLOMOWA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5969E437-BE71-4BF8-B52D-9AAF5796FE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E31816-D59A-4755-B2EF-4123E8D548D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A711F6BC-DA91-495B-A07B-FEE522077D34}"/>
+    <workbookView xWindow="6045" yWindow="0" windowWidth="21405" windowHeight="15330" xr2:uid="{A711F6BC-DA91-495B-A07B-FEE522077D34}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -147,10 +147,25 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -177,8 +192,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -530,7 +547,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,28 +612,37 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -627,12 +653,15 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -642,7 +671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
@@ -650,7 +679,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -658,23 +687,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>10</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>11</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -682,7 +717,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
@@ -690,7 +725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -698,7 +733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
@@ -706,7 +741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
@@ -714,15 +749,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>17</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>18</v>
       </c>
@@ -730,20 +768,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>19</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Made the final questionnaire
</commit_message>
<xml_diff>
--- a/questionnaire.xlsx
+++ b/questionnaire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\uczelnia\magister\PRACA DYPLOMOWA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E31816-D59A-4755-B2EF-4123E8D548D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C427E11-4849-4E8E-8C3E-6518D3364826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="0" windowWidth="21405" windowHeight="15330" xr2:uid="{A711F6BC-DA91-495B-A07B-FEE522077D34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A711F6BC-DA91-495B-A07B-FEE522077D34}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
   <si>
     <t>I lose track of time</t>
   </si>
@@ -141,6 +141,36 @@
   </si>
   <si>
     <t>Other thoughts</t>
+  </si>
+  <si>
+    <t>OG GEQ</t>
+  </si>
+  <si>
+    <t>I was fully occupied with the game</t>
+  </si>
+  <si>
+    <t>GEQ33-5</t>
+  </si>
+  <si>
+    <t>GEQ33-28</t>
+  </si>
+  <si>
+    <t>I was deeply concentrated in the game</t>
+  </si>
+  <si>
+    <t>I was interested in the game's story</t>
+  </si>
+  <si>
+    <t>GEQ33-3</t>
+  </si>
+  <si>
+    <t>I felt that I could explore things</t>
+  </si>
+  <si>
+    <t>I enjoyed it</t>
+  </si>
+  <si>
+    <t>GEQ33-20</t>
   </si>
 </sst>
 </file>
@@ -222,6 +252,20 @@
     <tableColumn id="3" xr3:uid="{F2E654B4-A3D0-4816-A653-36607DAB1DFF}" name="No"/>
     <tableColumn id="4" xr3:uid="{789B3513-B248-4AAB-A098-98A025DB83CB}" name="Maybe"/>
     <tableColumn id="5" xr3:uid="{6B4FF00B-7D52-4C83-A897-48590E78FF97}" name="Yes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AC091EA-67D1-4AAF-BFE2-49E2C6D58858}" name="Tabela32" displayName="Tabela32" ref="G9:K28" totalsRowShown="0">
+  <autoFilter ref="G9:K28" xr:uid="{3AC091EA-67D1-4AAF-BFE2-49E2C6D58858}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5D43B3EA-8FC9-4DBF-9809-5E2414E9366D}" name="Number"/>
+    <tableColumn id="2" xr3:uid="{8D7A1CC9-6089-4BC6-9776-7DD56E578046}" name="Question"/>
+    <tableColumn id="3" xr3:uid="{E3F4054B-D362-4D31-BB48-4651A345D324}" name="No"/>
+    <tableColumn id="4" xr3:uid="{40402C09-3B60-4FBC-B505-EFD79D733E19}" name="Maybe"/>
+    <tableColumn id="5" xr3:uid="{4262E0FA-9F2B-4D9D-A973-A1E22BE2389C}" name="Yes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -544,49 +588,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926F34D3-D9D3-4B99-AA8A-462924709E04}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -602,16 +653,37 @@
       <c r="E9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -621,8 +693,20 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -632,8 +716,17 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" s="2">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -643,16 +736,31 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" s="2">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>6</v>
       </c>
@@ -662,32 +770,62 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G15" s="2">
+        <v>6</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" s="2">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" s="2">
+        <v>8</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="2">
+        <v>9</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>10</v>
       </c>
@@ -697,94 +835,172 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="G19" s="2">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>11</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="G20" s="2">
+        <v>11</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>12</v>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>13</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="G22">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>14</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>14</v>
+      </c>
+      <c r="H23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>15</v>
       </c>
       <c r="B24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>15</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="G25">
+        <v>16</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>17</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="G26" s="2">
+        <v>17</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="G27">
+        <v>18</v>
+      </c>
+      <c r="H27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>19</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="G28" s="2">
+        <v>19</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -806,8 +1022,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>